<commit_message>
i added soem variables
</commit_message>
<xml_diff>
--- a/BUDGET PROBLEM.xlsx
+++ b/BUDGET PROBLEM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim oyinkansola\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim oyinkansola\OneDrive\Documents\BUDJET\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,19 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>BUDGET PROBLEM</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -50,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -58,14 +69,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -344,18 +369,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>